<commit_message>
excel onboarding parsing to onboard client model api added
</commit_message>
<xml_diff>
--- a/coachMe/Clientonboard.xlsx
+++ b/coachMe/Clientonboard.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasheora\Desktop\clients\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F9ECEC-9D0F-4E74-91F2-9095E825EEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="17490" windowHeight="12570"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Onboard Tab" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Goal (Lifestyle/Natural body building)</t>
   </si>
@@ -28,9 +22,6 @@
     <t>Full name</t>
   </si>
   <si>
-    <t>Contact details</t>
-  </si>
-  <si>
     <t>Sex</t>
   </si>
   <si>
@@ -46,33 +37,12 @@
     <t>Measurements(fill below in inches)</t>
   </si>
   <si>
-    <t>:Neck</t>
-  </si>
-  <si>
-    <t>:Shoulders</t>
-  </si>
-  <si>
-    <t>:chest</t>
-  </si>
-  <si>
-    <t>:Waist(around belly button)</t>
-  </si>
-  <si>
-    <t>:calves(right side)</t>
-  </si>
-  <si>
-    <t>:quads(right side)</t>
-  </si>
-  <si>
     <t>Daily activity level(Rate1-10)</t>
   </si>
   <si>
     <t>Is it possible for you to join gym?</t>
   </si>
   <si>
-    <t>current workout pattern or split</t>
-  </si>
-  <si>
     <t>Preferable workout timings</t>
   </si>
   <si>
@@ -107,9 +77,6 @@
   </si>
   <si>
     <t>Mention all the foods you can easily reach</t>
-  </si>
-  <si>
-    <t>Biggest food challenge(foods you dislike the most)</t>
   </si>
   <si>
     <t>Add pictures(front.Back.side)</t>
@@ -162,11 +129,35 @@
   <si>
     <t>Your current meals of the day</t>
   </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Neck</t>
+  </si>
+  <si>
+    <t>Shoulders</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Waist(around belly button)</t>
+  </si>
+  <si>
+    <t>Calves(right side)</t>
+  </si>
+  <si>
+    <t>Quads(right side)</t>
+  </si>
+  <si>
+    <t>Current workout pattern or split</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -507,17 +498,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.6640625" customWidth="1"/>
-    <col min="2" max="2" width="96.77734375" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="96.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -531,195 +522,247 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+      <c r="A3" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+      <c r="A9" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
+      <c r="A11" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
+      <c r="A12" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
+      <c r="A13" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
+      <c r="A14" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
+      <c r="A17" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
+      <c r="A32" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="19.2">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="35" spans="1:2" ht="19.5">
       <c r="A35" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="19.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="19.5">
       <c r="A36" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2" ht="19.2">
+    <row r="37" spans="1:2" ht="19.5">
       <c r="A37" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B37" s="5"/>
     </row>
-    <row r="38" spans="1:2" ht="19.2">
+    <row r="38" spans="1:2" ht="19.5">
       <c r="A38" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B38" s="5"/>
     </row>
-    <row r="39" spans="1:2" ht="19.2">
+    <row r="39" spans="1:2" ht="19.5">
       <c r="A39" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B39" s="5"/>
     </row>
-    <row r="40" spans="1:2" ht="19.2">
+    <row r="40" spans="1:2" ht="19.5">
       <c r="A40" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="16">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Type Correct Choice" error="Choice: &#10;Lifestyle&#10;Natural Body Building" sqref="B1">
+      <formula1>"Lifestyle, Natural Body Building"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Max length 30" sqref="B2">
+      <formula1>30</formula1>
+    </dataValidation>
+    <dataValidation type="custom" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Input!" error="Contact Number length is 10" promptTitle="Enter Your Contact Number" sqref="B3">
+      <formula1>AND(ISNUMBER(B3),LEN(B3)=10)</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Eneter correct Input" error="M for male&#10;F for female" prompt="M for Male&#10;F for Female" sqref="B4">
+      <formula1>"M,F"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter Age in Number" error="Enter Age in Number" promptTitle="Enter Age in Number" prompt="Enter Age in Number" sqref="B5">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter correct Input" promptTitle="Enter your height in Inches" sqref="B6">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter correct input" promptTitle="Enter your weight in KG" prompt="Enter your weight empty stomach morning" sqref="B7">
+      <formula1>300</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 B10 B13 B14">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B12">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter correct Input" error="It should be a number and between 0 to 10" sqref="B15">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Input" error="Enter value between 3 to 15" sqref="B19">
+      <formula1>3</formula1>
+      <formula2>15</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Input" error="Enter value between 0 to 10" sqref="B20">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Input" error="Enter Value between 0 to 10." sqref="B21">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Input Choice" sqref="B27">
+      <formula1>"N,V"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>